<commit_message>
changed ui components to be classes instead of methods in Screen class
</commit_message>
<xml_diff>
--- a/BMS/BMS Board/Exports/BMS Board BOM.xlsx
+++ b/BMS/BMS Board/Exports/BMS Board BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="236">
   <si>
     <t>Reference</t>
   </si>
@@ -85,7 +85,7 @@
     <t>https://www.mouser.com/Search/Refine.aspx?Keyword=581-08053C334KAT2A</t>
   </si>
   <si>
-    <t>&gt;  C2, C4-C13, C17</t>
+    <t>&gt;  C2, C4-C13, C17, C18</t>
   </si>
   <si>
     <t>0805ZC104MAT2A</t>
@@ -145,6 +145,30 @@
     <t>AVX - 08053C225K4T2A - SMD Multilayer Ceramic Capacitor, 2.2 uF, 25 V, 0805 [2012 Metric], +/- 10%, X7R</t>
   </si>
   <si>
+    <t>&gt;  D1, D2</t>
+  </si>
+  <si>
+    <t>S1G</t>
+  </si>
+  <si>
+    <t>DIOM5227X250N</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/S1M-D.pdf</t>
+  </si>
+  <si>
+    <t>ON Semi 400V 1A, Diode, 2-Pin DO-214AC S1G</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>512-S1G</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/ON-Semiconductor-Fairchild/S1G?qs=RJwZ8kJo1mjiLbqXClupXw%3D%3D</t>
+  </si>
+  <si>
     <t>&gt;  H1-H4</t>
   </si>
   <si>
@@ -157,6 +181,33 @@
     <t>~</t>
   </si>
   <si>
+    <t>&gt;  IC1, IC2</t>
+  </si>
+  <si>
+    <t>TLP2310_TPL,E</t>
+  </si>
+  <si>
+    <t>SOIC127P700X220-6N</t>
+  </si>
+  <si>
+    <t>https://componentsearchengine.com/Datasheets/1/TLP2310(TPL,E.pdf</t>
+  </si>
+  <si>
+    <t>High Speed Optocouplers Photo-IC 2.7-5.5V 3750Vrms 0.3mA 5Mb</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>TLP2310(TPL,E</t>
+  </si>
+  <si>
+    <t>757-TLP2310TPLE</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/Search/Refine.aspx?Keyword=757-TLP2310TPLE</t>
+  </si>
+  <si>
     <t>J1</t>
   </si>
   <si>
@@ -316,33 +367,6 @@
     <t>https://www.mouser.com/datasheet/2/143/201407061833256242-365628.pdf</t>
   </si>
   <si>
-    <t>O21</t>
-  </si>
-  <si>
-    <t>TLP2270_TP4,E</t>
-  </si>
-  <si>
-    <t>SOIC127P1105X220-8N</t>
-  </si>
-  <si>
-    <t>https://www.arrow.com/en/products/tlp2270-tp4e/toshiba</t>
-  </si>
-  <si>
-    <t>High Speed Optocouplers PHOTOCOUPLER GaAAs Infrared LED &amp; Photo IC</t>
-  </si>
-  <si>
-    <t>Toshiba</t>
-  </si>
-  <si>
-    <t>TLP2270(TP4,E</t>
-  </si>
-  <si>
-    <t>757-TLP2270TP4E</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/Toshiba/TLP2270TP4E?qs=byeeYqUIh0MfOygbGlY3Yg%3D%3D</t>
-  </si>
-  <si>
     <t>&gt;  P1-P6</t>
   </si>
   <si>
@@ -463,7 +487,7 @@
     <t>1 k</t>
   </si>
   <si>
-    <t>&gt;  R21-R40, R101, R120, R121</t>
+    <t>&gt;  R21-R40, R101, R102, R141, R142</t>
   </si>
   <si>
     <t>ERJ-S06F2002V</t>
@@ -505,7 +529,28 @@
     <t>https://www.mouser.com/Search/Refine.aspx?Keyword=279-CRGP2512F12R</t>
   </si>
   <si>
-    <t>&gt;  R102-R113</t>
+    <t>&gt;  R105-R108, R111-R114, R117-R128, R139, R140</t>
+  </si>
+  <si>
+    <t>ERJ-S06J472V</t>
+  </si>
+  <si>
+    <t>https://componentsearchengine.com/Datasheets/1/ERJ-S06J472V.pdf</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 0805 4.7Kohms 5% Anti-Sulfur</t>
+  </si>
+  <si>
+    <t>667-ERJ-S06J472V</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/Search/Refine.aspx?Keyword=667-ERJ-S06J472V</t>
+  </si>
+  <si>
+    <t>4.7 k</t>
+  </si>
+  <si>
+    <t>&gt;  R103, R104, R109, R110, R115, R116, R129-R134</t>
   </si>
   <si>
     <t>ERJ-UP6J103v</t>
@@ -529,7 +574,25 @@
     <t>10 k</t>
   </si>
   <si>
-    <t>&gt;  R114, R115</t>
+    <t>&gt;  R135, R138</t>
+  </si>
+  <si>
+    <t>ERJ-P06F2200V</t>
+  </si>
+  <si>
+    <t>https://componentsearchengine.com/Datasheets/1/ERJ-P06F2200V.pdf</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 0805 220ohms 0.5W 1% AEC-Q200</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F2200V</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/Search/Refine.aspx?Keyword=667-ERJ-P06F2200V</t>
+  </si>
+  <si>
+    <t>&gt;  R136, R137</t>
   </si>
   <si>
     <t>ERJ-6ENF5600V</t>
@@ -545,45 +608,6 @@
   </si>
   <si>
     <t>https://www.mouser.com/Search/Refine.aspx?Keyword=667-ERJ-6ENF5600V</t>
-  </si>
-  <si>
-    <t>&gt;  R116, R117</t>
-  </si>
-  <si>
-    <t>ERJ-P06F2200V</t>
-  </si>
-  <si>
-    <t>https://componentsearchengine.com/Datasheets/1/ERJ-P06F2200V.pdf</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 0805 220ohms 0.5W 1% AEC-Q200</t>
-  </si>
-  <si>
-    <t>667-ERJ-P06F2200V</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/Search/Refine.aspx?Keyword=667-ERJ-P06F2200V</t>
-  </si>
-  <si>
-    <t>&gt;  R118, R119</t>
-  </si>
-  <si>
-    <t>ERJ-S06J472V</t>
-  </si>
-  <si>
-    <t>https://componentsearchengine.com/Datasheets/1/ERJ-S06J472V.pdf</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 0805 4.7Kohms 5% Anti-Sulfur</t>
-  </si>
-  <si>
-    <t>667-ERJ-S06J472V</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/Search/Refine.aspx?Keyword=667-ERJ-S06J472V</t>
-  </si>
-  <si>
-    <t>4.7 k</t>
   </si>
   <si>
     <t>&gt;  U1-U20</t>
@@ -902,7 +926,7 @@
         <v>31</v>
       </c>
       <c r="O3" s="3">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="4">
@@ -984,47 +1008,52 @@
       <c r="C6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="G6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="O6" s="3">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="3">
-        <v>2.41</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="6"/>
       <c r="O7" s="3">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
@@ -1044,48 +1073,48 @@
         <v>60</v>
       </c>
       <c r="H8" s="3">
-        <v>10.795</v>
+        <v>2.2</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>61</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O8" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>71</v>
@@ -1110,59 +1139,59 @@
       <c r="D10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3">
+        <v>10.795</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="O10" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="5"/>
       <c r="G11" s="3" t="s">
         <v>85</v>
       </c>
       <c r="H11" s="3">
-        <v>5.5</v>
+        <v>25.0</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>86</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O11" s="3">
         <v>1.0</v>
@@ -1170,159 +1199,168 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="L12" s="5"/>
+      <c r="K12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="O12" s="3">
-        <v>22.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L13" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="G13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="O13" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="L14" s="5"/>
       <c r="O14" s="3">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H15" s="3">
-        <v>2.2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>109</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="6"/>
       <c r="O15" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="O16" s="3">
-        <v>6.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="3">
-        <v>4.30452221E8</v>
+        <v>118</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D17" s="5"/>
       <c r="L17" s="5"/>
       <c r="O17" s="3">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4.30452221E8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H18" s="3">
-        <v>2.52</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N18" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="D18" s="6"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="6"/>
+      <c r="N18" s="3"/>
       <c r="O18" s="3">
         <v>1.0</v>
       </c>
@@ -1335,31 +1373,31 @@
         <v>124</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3">
+        <v>2.52</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="J19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="O19" s="3">
         <v>1.0</v>
@@ -1367,33 +1405,36 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="N20" s="3" t="s">
         <v>139</v>
       </c>
       <c r="O20" s="3">
@@ -1405,66 +1446,69 @@
         <v>140</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="L21" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="O21" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>149</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="3"/>
       <c r="O22" s="3">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>152</v>
@@ -1476,33 +1520,33 @@
         <v>0.7</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O23" s="3">
-        <v>23.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>160</v>
@@ -1511,13 +1555,13 @@
         <v>161</v>
       </c>
       <c r="H24" s="3">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>162</v>
@@ -1525,49 +1569,49 @@
       <c r="L24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="M24" s="3">
-        <v>12.0</v>
+      <c r="M24" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="O24" s="3">
-        <v>60.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="K25" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="M25" s="3" t="s">
         <v>171</v>
       </c>
+      <c r="M25" s="3">
+        <v>12.0</v>
+      </c>
       <c r="O25" s="3">
-        <v>12.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="26">
@@ -1578,7 +1622,7 @@
         <v>173</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>174</v>
@@ -1590,7 +1634,7 @@
         <v>0.7</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>173</v>
@@ -1601,84 +1645,84 @@
       <c r="L26" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="M26" s="3">
-        <v>560.0</v>
+      <c r="M26" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="O26" s="3">
-        <v>2.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H27" s="3">
         <v>0.7</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="M27" s="3">
-        <v>220.0</v>
+        <v>185</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="O27" s="3">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H28" s="3">
         <v>0.7</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
+      </c>
+      <c r="M28" s="3">
+        <v>220.0</v>
       </c>
       <c r="O28" s="3">
         <v>2.0</v>
@@ -1686,153 +1730,156 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="K29" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="M29" s="3">
+        <v>560.0</v>
       </c>
       <c r="O29" s="3">
-        <v>20.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H30" s="3">
-        <v>1.12</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="K30" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="O30" s="3">
-        <v>4.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1.12</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="H31" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="K31" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="O31" s="3">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="K32" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="O32" s="3">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>222</v>
@@ -1841,27 +1888,58 @@
         <v>223</v>
       </c>
       <c r="H33" s="3">
-        <v>2.65</v>
+        <v>1.75</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>224</v>
       </c>
       <c r="J33" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="O33" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="O33" s="3">
+      <c r="B34" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2.65</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="O34" s="3">
         <v>3.0</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="D34" s="5"/>
-      <c r="L34" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1871,29 +1949,29 @@
     <hyperlink r:id="rId4" ref="L3"/>
     <hyperlink r:id="rId5" ref="D4"/>
     <hyperlink r:id="rId6" ref="L4"/>
-    <hyperlink r:id="rId7" ref="D7"/>
-    <hyperlink r:id="rId8" ref="L7"/>
+    <hyperlink r:id="rId7" ref="D6"/>
+    <hyperlink r:id="rId8" ref="L6"/>
     <hyperlink r:id="rId9" ref="D8"/>
     <hyperlink r:id="rId10" ref="L8"/>
     <hyperlink r:id="rId11" ref="D9"/>
     <hyperlink r:id="rId12" ref="L9"/>
     <hyperlink r:id="rId13" ref="D10"/>
     <hyperlink r:id="rId14" ref="L10"/>
-    <hyperlink r:id="rId15" ref="L11"/>
-    <hyperlink r:id="rId16" ref="D12"/>
-    <hyperlink r:id="rId17" ref="D13"/>
-    <hyperlink r:id="rId18" ref="D14"/>
-    <hyperlink r:id="rId19" ref="D15"/>
-    <hyperlink r:id="rId20" ref="L15"/>
-    <hyperlink r:id="rId21" ref="D18"/>
-    <hyperlink r:id="rId22" ref="L18"/>
+    <hyperlink r:id="rId15" ref="D11"/>
+    <hyperlink r:id="rId16" ref="L11"/>
+    <hyperlink r:id="rId17" ref="D12"/>
+    <hyperlink r:id="rId18" ref="L12"/>
+    <hyperlink r:id="rId19" ref="L13"/>
+    <hyperlink r:id="rId20" ref="D14"/>
+    <hyperlink r:id="rId21" ref="D15"/>
+    <hyperlink r:id="rId22" ref="D16"/>
     <hyperlink r:id="rId23" ref="D19"/>
     <hyperlink r:id="rId24" ref="L19"/>
     <hyperlink r:id="rId25" ref="D20"/>
     <hyperlink r:id="rId26" ref="L20"/>
     <hyperlink r:id="rId27" ref="D21"/>
-    <hyperlink r:id="rId28" ref="D22"/>
-    <hyperlink r:id="rId29" ref="L22"/>
+    <hyperlink r:id="rId28" ref="L21"/>
+    <hyperlink r:id="rId29" ref="D22"/>
     <hyperlink r:id="rId30" ref="D23"/>
     <hyperlink r:id="rId31" ref="L23"/>
     <hyperlink r:id="rId32" ref="D24"/>
@@ -1916,7 +1994,9 @@
     <hyperlink r:id="rId49" ref="L32"/>
     <hyperlink r:id="rId50" ref="D33"/>
     <hyperlink r:id="rId51" ref="L33"/>
+    <hyperlink r:id="rId52" ref="D34"/>
+    <hyperlink r:id="rId53" ref="L34"/>
   </hyperlinks>
-  <drawing r:id="rId52"/>
+  <drawing r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>